<commit_message>
Added converter (fix int cell issue)
</commit_message>
<xml_diff>
--- a/spec/fixtures/valid.xlsx
+++ b/spec/fixtures/valid.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t xml:space="preserve">Phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column with int</t>
   </si>
   <si>
     <t xml:space="preserve">Jean</t>
@@ -185,16 +188,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.76"/>
@@ -216,39 +219,48 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -273,7 +285,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -281,7 +293,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>